<commit_message>
run all test cases successfully and modified data file
</commit_message>
<xml_diff>
--- a/EnrollMultipleLearners.xlsx
+++ b/EnrollMultipleLearners.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>learnerid</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>enddate</t>
+  </si>
+  <si>
+    <t>2021-09-07</t>
+  </si>
+  <si>
+    <t>2022-06-07</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,7 +376,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,16 +385,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -399,11 +405,11 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>44324</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44656</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -413,11 +419,11 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>44324</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44656</v>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -427,11 +433,11 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
-        <v>44324</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44656</v>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -441,15 +447,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>44324</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44656</v>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>